<commit_message>
Conexao entre receitas, receitas cadastradas e banco de dados (excel)
</commit_message>
<xml_diff>
--- a/data/receitas.xlsx
+++ b/data/receitas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,86 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>[teste] Frango ao molho de queijos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>File de peito de frango</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>300</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>[teste] Frango ao molho de queijos</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Arroz Parboilizado</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>150</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Un</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>[teste] Frango ao molho de queijos</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Queijo Mussarela fatiado</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>[teste] Frango ao molho de queijos</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Queijo Parmesao</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Subindo arquivo de receitas atualizado
</commit_message>
<xml_diff>
--- a/data/receitas.xlsx
+++ b/data/receitas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\estancia_dos_ventos\ambiente_virtual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96A9829-92E8-4B6B-9287-45F679EF30F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC3E7A1-9D41-4315-94A8-8F706CEB13BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1980" windowWidth="16995" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>prato</t>
   </si>
@@ -39,9 +39,6 @@
     <t>unidade</t>
   </si>
   <si>
-    <t>[TESTE] Strogonoff do Chefe</t>
-  </si>
-  <si>
     <t>File de peito de frango</t>
   </si>
   <si>
@@ -54,37 +51,13 @@
     <t>creme de leite</t>
   </si>
   <si>
-    <t>[teste] Frango ao molho de queijos</t>
-  </si>
-  <si>
-    <t>Queijo Mussarela fatiado</t>
-  </si>
-  <si>
-    <t>Kg</t>
-  </si>
-  <si>
-    <t>Queijo Parmesao</t>
-  </si>
-  <si>
-    <t>Prato do chefe - teste número 05</t>
-  </si>
-  <si>
-    <t>Alho Poro</t>
-  </si>
-  <si>
-    <t>Bife do Vazio</t>
-  </si>
-  <si>
-    <t>Batata frita corte fino</t>
-  </si>
-  <si>
-    <t>Cebola Roxa</t>
-  </si>
-  <si>
     <t>Batata Palha</t>
   </si>
   <si>
     <t>Cogumelo champignon</t>
+  </si>
+  <si>
+    <t>Strogonoff do Chefe</t>
   </si>
 </sst>
 </file>
@@ -447,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,198 +450,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
         <v>5</v>
-      </c>
-      <c r="C7">
-        <v>300</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>150</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>300</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>148</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>101</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterando novamente a receita principal
</commit_message>
<xml_diff>
--- a/data/receitas.xlsx
+++ b/data/receitas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\estancia_dos_ventos\ambiente_virtual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC3E7A1-9D41-4315-94A8-8F706CEB13BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6557E621-ACA6-4142-B787-63F2B43E2BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>Cogumelo champignon</t>
   </si>
   <si>
-    <t>Strogonoff do Chefe</t>
+    <t>Strogonoff do Frango</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Zerando os arquivos de estoque e receita para iniciarem do zero
</commit_message>
<xml_diff>
--- a/data/receitas.xlsx
+++ b/data/receitas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus\estancia_dos_ventos\ambiente_virtual\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6557E621-ACA6-4142-B787-63F2B43E2BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B91BBB-DE5E-443E-8124-1DE578DBAEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2325" windowWidth="16995" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>prato</t>
   </si>
@@ -37,27 +37,6 @@
   </si>
   <si>
     <t>unidade</t>
-  </si>
-  <si>
-    <t>File de peito de frango</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Arroz Parboilizado</t>
-  </si>
-  <si>
-    <t>creme de leite</t>
-  </si>
-  <si>
-    <t>Batata Palha</t>
-  </si>
-  <si>
-    <t>Cogumelo champignon</t>
-  </si>
-  <si>
-    <t>Strogonoff do Frango</t>
   </si>
 </sst>
 </file>
@@ -420,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A6" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,76 +427,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>160</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>80</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>